<commit_message>
add details and citations to data sources tbls
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_datasources.xlsx
+++ b/scenario_analysis_v2/scenariov2_datasources.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>none (all data present in useeior package)</t>
   </si>
@@ -159,9 +159,6 @@
     <t>multiple</t>
   </si>
   <si>
-    <t>Data from Appendices 3-5 of 2015-2020 Dietary Guidelines for Americans, manually copied and saved to CSV</t>
-  </si>
-  <si>
     <t>https://www.dietaryguidelines.gov/sites/default/files/2019-05/2015-2020_Dietary_Guidelines.pdf</t>
   </si>
   <si>
@@ -223,6 +220,63 @@
   </si>
   <si>
     <t>Data on crop and livestock production value and weight, and area harvested, by state and county</t>
+  </si>
+  <si>
+    <t>Data from Appendices 3-5 of 2015-2020 Dietary Guidelines for Americans, manually copied and saved to CSV (calories per day or servings per day of each food group on recommended diets)</t>
+  </si>
+  <si>
+    <t>Data copied directly from report and saved to CSV (calories per day of each food group on planetary health diet)</t>
+  </si>
+  <si>
+    <t>Relative percentage losses for ~200 food items at different stages of the food supply chain, and the total amount of each food item available for consumption per capita daily in the USA, in units of calories and servings</t>
+  </si>
+  <si>
+    <t>Relative prices per unit weight for ~40 food items averaged across different regions of the USA</t>
+  </si>
+  <si>
+    <t>Total personal income of each USA county</t>
+  </si>
+  <si>
+    <t>Potential species lost per unit of land converted to human use, across ecoregions, taxa, and land use types</t>
+  </si>
+  <si>
+    <t>Number of establishments, employees, and total payroll for industries classified by NAICS code for each USA county</t>
+  </si>
+  <si>
+    <t>Number of establishments, employees, payroll, and total receipts for industries classified by NAICS code for each USA state</t>
+  </si>
+  <si>
+    <t>Update when the paper is published, otherwise use Yang et al. citation</t>
+  </si>
+  <si>
+    <t>Buzby, J.C., Farah-Wells, H., Hyman, J., 2014. The estimated amount, value, and calories of postharvest food losses at the retail and consumer levels in the United States. SSRN Electronic Journal. https://doi.org/10.2139/ssrn.2501659</t>
+  </si>
+  <si>
+    <t>Chaudhary, A., Brooks, T.M., 2018. Land use intensity-specific global characterization factors to assess product biodiversity footprints. Environ. Sci. Technol. 52, 5094–5104. https://doi.org/10.1021/acs.est.7b05570</t>
+  </si>
+  <si>
+    <t>USDA Economic Research Service, 2019. Quarterly Food-at-Home Price Database [WWW Document]. URL https://www.ers.usda.gov/data-products/quarterly-food-at-home-price-database/ (accessed 8.5.20).</t>
+  </si>
+  <si>
+    <t>USDA - National Agricultural Statistics Service - 2012 Census of Agriculture - Volume 1, Chapter 1: U.S. National Level Data [WWW Document], n.d. URL https://www.nass.usda.gov/Publications/AgCensus/2012/Full_Report/Volume_1,_Chapter_1_US/ (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, 2014. County Business Patterns: 2012 [WWW Document]. The United States Census Bureau. URL https://www.census.gov/data/datasets/2012/econ/cbp/2012-cbp.html (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, 2015. SUSB Datasets [WWW Document]. The United States Census Bureau. URL https://www.census.gov/programs-surveys/susb/data/datasets.html (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>U.S. Department of Health and Human Services, U.S. Department of Agriculture, 2015. 2015-2020 Dietary Guidelines for Americans, 8th Edition [WWW Document]. URL http://health.gov/dietaryguidelines/2015/guidelines (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>Willett, W., Rockström, J., Loken, B., Springmann, M., Lang, T., Vermeulen, S., Garnett, T., Tilman, D., DeClerck, F., Wood, A., Jonell, M., Clark, M., Gordon, L.J., Fanzo, J., Hawkes, C., Zurayk, R., Rivera, J.A., De Vries, W., Majele Sibanda, L., Afshin, A., Chaudhary, A., Herrero, M., Agustina, R., Branca, F., Lartey, A., Fan, S., Crona, B., Fox, E., Bignet, V., Troell, M., Lindahl, T., Singh, S., Cornell, S.E., Srinath Reddy, K., Narain, S., Nishtar, S., Murray, C.J.L., 2019. Food in the Anthropocene: the EAT–Lancet Commission on healthy diets from sustainable food systems. The Lancet 393, 447–492. https://doi.org/10.1016/S0140-6736(18)31788-4</t>
+  </si>
+  <si>
+    <t>FAO (Food and Agriculture Organization of the United Nations)), 2021. FAOSTAT [WWW Document]. URL http://www.fao.org/faostat/en/#home (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>U.S. Bureau of Economic Analysis (BEA), 2021. Regional Data: GDP &amp; Personal Income [WWW Document]. URL https://apps.bea.gov/iTable/index_regional.cfm (accessed 4.1.21).</t>
   </si>
 </sst>
 </file>
@@ -267,12 +321,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,14 +615,16 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="46" customWidth="1"/>
+    <col min="1" max="1" width="46" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -574,13 +634,13 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -599,24 +659,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C2">
         <v>2012</v>
       </c>
-      <c r="D2" t="s">
-        <v>64</v>
+      <c r="D2" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2">
         <v>44278</v>
@@ -624,25 +684,28 @@
       <c r="H2" s="2">
         <v>44278</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C3">
         <v>2012</v>
       </c>
-      <c r="D3" t="s">
-        <v>65</v>
+      <c r="D3" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2">
         <v>43762</v>
@@ -650,22 +713,28 @@
       <c r="H3" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C4">
         <v>2012</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="2">
         <v>43507</v>
@@ -673,22 +742,28 @@
       <c r="H4" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
+      <c r="D5" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="2">
         <v>43507</v>
@@ -696,25 +771,28 @@
       <c r="H5" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>44</v>
+      <c r="D6" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="2">
         <v>44172</v>
@@ -722,22 +800,28 @@
       <c r="H6" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
+      <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="2">
         <v>44173</v>
@@ -745,22 +829,28 @@
       <c r="H7" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
       </c>
+      <c r="D8" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2">
         <v>44174</v>
@@ -768,22 +858,28 @@
       <c r="H8" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C9">
         <v>2010</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" s="2">
         <v>43538</v>
@@ -791,22 +887,25 @@
       <c r="H9" s="2">
         <v>44285</v>
       </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -817,56 +916,72 @@
       <c r="H10" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C11">
         <v>2012</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>52</v>
       </c>
       <c r="H11" s="2">
         <v>44285</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>43</v>
       </c>
+      <c r="D12" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="2">
         <v>44172</v>
       </c>
       <c r="H12" s="2">
         <v>44285</v>
+      </c>
+      <c r="I12" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F12" r:id="rId1"/>
+    <hyperlink ref="F11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fill out crosswalks tab of data sources spreadsheet
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_datasources.xlsx
+++ b/scenario_analysis_v2/scenariov2_datasources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="124">
   <si>
     <t>none (all data present in useeior package)</t>
   </si>
@@ -66,9 +66,6 @@
     <t xml:space="preserve">raw_data/USDA/2012_cdqt_data.txt; </t>
   </si>
   <si>
-    <t>crosswalk_tables/wt_per_bushel.csv; crosswalk_tables/crop_priceperunit_20142016.csv</t>
-  </si>
-  <si>
     <t>useeio2012v2.0_NAICS_BEA_crosswalk.csv</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>raw_data/Census/SUSB/us_state_6digitnaics_2012.txt</t>
   </si>
   <si>
-    <t>lafa_dietary_guidelines_crosswalk.csv;</t>
-  </si>
-  <si>
     <t>raw_data/commodity_flows/Lin_supp_info/County Personal Income.xlsx</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>crossreference_tables/fao_prodcodes_harmonized_fbs.csv</t>
   </si>
   <si>
-    <t>qfahpd_lafa_crosswalk.csv; lafa_qfahpd_naics.csv; lafa_category_structure.csv; bea_lafa_crosswalk.csv</t>
-  </si>
-  <si>
     <t>raw_data/food_consumption/diet_guidelines/lancet_planetary_health_diet.csv</t>
   </si>
   <si>
@@ -277,6 +268,135 @@
   </si>
   <si>
     <t>U.S. Bureau of Economic Analysis (BEA), 2021. Regional Data: GDP &amp; Personal Income [WWW Document]. URL https://apps.bea.gov/iTable/index_regional.cfm (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>Crosswalk description</t>
+  </si>
+  <si>
+    <t>Name of file</t>
+  </si>
+  <si>
+    <t>lafa_qfahpd_naics.csv</t>
+  </si>
+  <si>
+    <t>lafa_category_structure.csv</t>
+  </si>
+  <si>
+    <t>bea_lafa_crosswalk.csv</t>
+  </si>
+  <si>
+    <t>qfahpd_lafa_crosswalk.csv</t>
+  </si>
+  <si>
+    <t>crossreference_tables/lafa_dietary_guidelines_crosswalk.csv</t>
+  </si>
+  <si>
+    <t>Created manually or downloaded?</t>
+  </si>
+  <si>
+    <t>downloaded</t>
+  </si>
+  <si>
+    <t>created manually</t>
+  </si>
+  <si>
+    <t>Details/purpose</t>
+  </si>
+  <si>
+    <t>BEA codes to LAFA food categories</t>
+  </si>
+  <si>
+    <t>LAFA category hierarchical structure</t>
+  </si>
+  <si>
+    <t>LAFA food categories to QFAHPD food categories to BEA codes</t>
+  </si>
+  <si>
+    <t>QFAHPD food categories to LAFA food categories</t>
+  </si>
+  <si>
+    <t>FAOSTAT commodity codes to FAO food balance sheet commodity codes</t>
+  </si>
+  <si>
+    <t>FAOSTAT commodity codes in trade dataset to FAOSTAT commodity codes in production dataset</t>
+  </si>
+  <si>
+    <t>LAFA food categories to Lancet and USDA dietary guidelines food groups</t>
+  </si>
+  <si>
+    <t>NAICS codes to BEA codes</t>
+  </si>
+  <si>
+    <t>FAOSTAT category hierarchical structure</t>
+  </si>
+  <si>
+    <t>Identifies which FAOSTAT codes represent aggregations of individual items. Aggregates are removed from analysis.</t>
+  </si>
+  <si>
+    <t>Identifies which LAFA food groups represent aggregations of individual items. Aggregates are removed from analysis.</t>
+  </si>
+  <si>
+    <t>Harmonizes NAICS2012 codes (used in NASS Census of Agriculture, SUSB, and CBP datasets) with BEA codes (used in input-output tables). Typically many-to-one NAICS-BEA mapping</t>
+  </si>
+  <si>
+    <t>Maps LAFA foods to dietary guideline food groups for Lancet and USDA diets so that waste and diet scenarios can be combined. Typically many-to-one LAFA-diet mapping</t>
+  </si>
+  <si>
+    <t>Weight in pounds per bushel of grain and oilseed crops</t>
+  </si>
+  <si>
+    <t>Price per bushel or hundredweight of grain and oilseed crops in 2014-2016</t>
+  </si>
+  <si>
+    <t>crossreference_tables/wt_per_bushel.csv</t>
+  </si>
+  <si>
+    <t>crossreference_tables/crop_priceperunit_20142016.csv</t>
+  </si>
+  <si>
+    <t>For converting grain and oilseed production value to weight, to disaggregate grain from oilseed production values</t>
+  </si>
+  <si>
+    <t>URL if applicable</t>
+  </si>
+  <si>
+    <t>Harmonizes QFAHPD food categories with LAFA food categories, used to convert loss rates by weight to loss rates by monetary value. Typically one-to-many mapping QFAHPD to LAFA.</t>
+  </si>
+  <si>
+    <t>Harmonizes LAFA to QFAHPD to BEA codes, used to convert loss rates by weight to monetary value. Typically one-to-many mapping for QFAHPD-LAFA and QFAHPD-BEA.</t>
+  </si>
+  <si>
+    <t>Harmonizes BEA codes to LAFA food categories. Typically one-to-many mapping BEA-LAFA. Used to convert scenario consumption factors for LAFA categories to BEA codes.</t>
+  </si>
+  <si>
+    <t>https://www.rayglen.com/crop-bushel-weights/</t>
+  </si>
+  <si>
+    <t>https://www.nass.usda.gov/Publications/Todays_Reports/reports/cpvl0217.pdf</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Rayglen</t>
+  </si>
+  <si>
+    <t>USDA Economic Research Service</t>
+  </si>
+  <si>
+    <t>http://www.fao.org/faostat/en/#data/BC/metadata</t>
+  </si>
+  <si>
+    <t>FAOSTAT</t>
+  </si>
+  <si>
+    <t>U.S. EPA USEEIO model (useeior package)</t>
+  </si>
+  <si>
+    <t>Harmonizes the FAOSTAT codes in the crop and livestock production data by country with the codes in the international trade data, used to determine the proportion of each product exported to the United States</t>
+  </si>
+  <si>
+    <t>Harmonizes the FAOSTAT codes in the crop and livestock production data by country with the food balance sheet commodity codes, used to determine the proportion of each crop that is used for feed that feeds livestock exported to the United States</t>
   </si>
 </sst>
 </file>
@@ -614,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -635,10 +755,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -661,22 +781,22 @@
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <v>2012</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G2" s="2">
         <v>44278</v>
@@ -685,27 +805,27 @@
         <v>44278</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>2012</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G3" s="2">
         <v>43762</v>
@@ -714,27 +834,27 @@
         <v>44285</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>2012</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2">
         <v>43507</v>
@@ -743,27 +863,27 @@
         <v>44285</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2">
         <v>43507</v>
@@ -772,27 +892,27 @@
         <v>44285</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2">
         <v>44172</v>
@@ -801,27 +921,27 @@
         <v>44285</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G7" s="2">
         <v>44173</v>
@@ -830,27 +950,27 @@
         <v>44285</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" s="2">
         <v>44174</v>
@@ -859,27 +979,27 @@
         <v>44285</v>
       </c>
       <c r="I8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>2010</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2">
         <v>43538</v>
@@ -888,24 +1008,24 @@
         <v>44285</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -917,56 +1037,56 @@
         <v>44285</v>
       </c>
       <c r="I10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>2012</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H11" s="2">
         <v>44285</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G12" s="2">
         <v>44172</v>
@@ -975,7 +1095,7 @@
         <v>44285</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -989,47 +1109,215 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="5" width="19.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
combine nonspatial and spatial data source table into one
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_datasources.xlsx
+++ b/scenario_analysis_v2/scenariov2_datasources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="180">
   <si>
     <t>none (all data present in useeior package)</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Name of file(s)</t>
-  </si>
-  <si>
     <t>Location on web</t>
   </si>
   <si>
@@ -63,15 +60,9 @@
     <t>raw_data/FAOSTAT/faostat_item_group_lookup.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">raw_data/USDA/2012_cdqt_data.txt; </t>
-  </si>
-  <si>
     <t>useeio2012v2.0_NAICS_BEA_crosswalk.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">raw_data/Census/CBP/cbp12co.txt; </t>
-  </si>
-  <si>
     <t>raw_data/Census/SUSB/us_state_6digitnaics_2012.txt</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>https://www.ers.usda.gov/data-products/food-availability-per-capita-data-system/</t>
   </si>
   <si>
-    <t xml:space="preserve">Supplementary information from Lin et al. 2019, derived from U.S. </t>
-  </si>
-  <si>
     <t>https://apps.bea.gov/iTable/iTable.cfm?reqid=70&amp;step=1&amp;acrdn=6</t>
   </si>
   <si>
@@ -397,13 +385,193 @@
   </si>
   <si>
     <t>Harmonizes the FAOSTAT codes in the crop and livestock production data by country with the food balance sheet commodity codes, used to determine the proportion of each crop that is used for feed that feeds livestock exported to the United States</t>
+  </si>
+  <si>
+    <t>Supplementary information from Lin et al. 2019, derived from U.S. Bureau of Economic Analysis</t>
+  </si>
+  <si>
+    <t>raw_data/USDA/2012_cdqt_data.txt</t>
+  </si>
+  <si>
+    <t>raw_data/Census/CBP/cbp12co.txt</t>
+  </si>
+  <si>
+    <t>Name of file(s) archived in manuscript data repository</t>
+  </si>
+  <si>
+    <t>SPATIAL DATA</t>
+  </si>
+  <si>
+    <t>The Nature Conservancy terrestrial ecoregions</t>
+  </si>
+  <si>
+    <t>The Nature Conservancy</t>
+  </si>
+  <si>
+    <t>Polygon file with all boundaries of terrestrial ecoregions globally</t>
+  </si>
+  <si>
+    <t>tnc_terr_ecoregions.shp (ESRI shapefile with multiple files)</t>
+  </si>
+  <si>
+    <t>http://maps.tnc.org/gis_data.html</t>
+  </si>
+  <si>
+    <t>Olson, D. M. and E. Dinerstein. 2002. The Global 200: Priority ecoregions for global conservation. (PDF file) Annals of the Missouri Botanical Garden 89:125-126.</t>
+  </si>
+  <si>
+    <t>United States administrative boundaries shapefile</t>
+  </si>
+  <si>
+    <t>Global Administrative Areas Database</t>
+  </si>
+  <si>
+    <t>Polygon file of the United States' country boundaries based on GADM v2.0</t>
+  </si>
+  <si>
+    <t>USA_adm0.shp (ESRI shapefile with multiple files)</t>
+  </si>
+  <si>
+    <t>No longer available. The most recent version is available at https://gadm.org/download_country_v3.html</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>GADM (Global Administrative Areas Database) [WWW Document], n.d. URL https://gadm.org/ (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>United States county boundaries shapefile</t>
+  </si>
+  <si>
+    <t>Polygon file of the United States county boundaries as they existed in 2014</t>
+  </si>
+  <si>
+    <t>cb_2014_us_county_500k.shp (ESRI shapefile with multiple files)</t>
+  </si>
+  <si>
+    <t>No longer available. A similar file is available at https://www2.census.gov/geo/tiger/TIGER2014/COUNTY/</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, n.d. TIGER/Line Shapefiles [WWW Document]. The United States Census Bureau. URL https://www.census.gov/geographies/mapping-files/time-series/geo/tiger-line-file.html (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>Global country administrative boundaries shapefile</t>
+  </si>
+  <si>
+    <t>Natural Earth</t>
+  </si>
+  <si>
+    <t>Polygon file of all country boundaries as they existed in 2018</t>
+  </si>
+  <si>
+    <t>ne_50m_admin_0_countries.shp (ESRI shapefile with multiple files)</t>
+  </si>
+  <si>
+    <t>https://www.naturalearthdata.com/downloads/50m-cultural-vectors/</t>
+  </si>
+  <si>
+    <t>Natural Earth - Free vector and raster map data at 1:10m, 1:50m, and 1:110m scales, n.d. URL https://www.naturalearthdata.com/ (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>National Land Cover Database 2016, CONUS</t>
+  </si>
+  <si>
+    <t>Multresolution Land Characteristics Consortium</t>
+  </si>
+  <si>
+    <t>Raster at 30m resolution of modeled land cover classes in contiguous United States</t>
+  </si>
+  <si>
+    <t>NLCD_2016_Land_Cover_L48_20190424.img</t>
+  </si>
+  <si>
+    <t>https://www.mrlc.gov/data</t>
+  </si>
+  <si>
+    <t>Dewitz, J., 2019, National Land Cover Database (NLCD) 2016 Products: U.S. Geological Survey data release, https://doi.org/10.5066/P96HHBIE.</t>
+  </si>
+  <si>
+    <t>National Land Cover Database 2016, Alaska</t>
+  </si>
+  <si>
+    <t>Raster at 30m resolution of modeled land cover classes in Alaska</t>
+  </si>
+  <si>
+    <t>NLCD_2016_Land_Cover_AK_20200724.img</t>
+  </si>
+  <si>
+    <t>https://www.mrlc.gov/data/nlcd-2016-land-cover-alaska</t>
+  </si>
+  <si>
+    <t>NOAA Land Cover Dataset 2001, Hawaii</t>
+  </si>
+  <si>
+    <t>Raster at 30m resolution of modeled land cover classes in Hawaii</t>
+  </si>
+  <si>
+    <t>hi_landcover_wimperv_9-30-08_se5.img</t>
+  </si>
+  <si>
+    <t>https://www.mrlc.gov/data/nlcd-2001-land-cover-hawaii-0</t>
+  </si>
+  <si>
+    <t>MRLC, 2003. NLCD 2001 Land Cover (HAWAII) | Multi-Resolution Land Characteristics (MRLC) Consortium [WWW Document]. URL https://www.mrlc.gov/data/nlcd-2001-land-cover-hawaii-0 (accessed 4.1.21).</t>
+  </si>
+  <si>
+    <t>Global Agricultural Lands: Pastures v1</t>
+  </si>
+  <si>
+    <t>SEDAC CIESIN, Columbia University</t>
+  </si>
+  <si>
+    <t>Raster at 1km resolution of global pastureland</t>
+  </si>
+  <si>
+    <t>pasture.tif</t>
+  </si>
+  <si>
+    <t>https://sedac.ciesin.columbia.edu/data/set/aglands-pastures-2000/data-download</t>
+  </si>
+  <si>
+    <t>Ramankutty, N., Evan, A.T., Monfreda, C., Foley, J.A., 2008. Farming the planet: 1. Geographic distribution of global agricultural lands in the year 2000. Global Biogeochemical Cycles 22. https://doi.org/10.1029/2007GB002952</t>
+  </si>
+  <si>
+    <t>Global Food Security Support Analysis Data (GFSAD) Crop Dominance 2010 Global 1 km</t>
+  </si>
+  <si>
+    <t>Raster at 1km resolution of global irrigated and rainfed cropland</t>
+  </si>
+  <si>
+    <t>GFSAD1KCD.2010.001.2016348142525.tif</t>
+  </si>
+  <si>
+    <t>https://www.usgs.gov/centers/wgsc/science/global-food-security-support-analysis-data-30-m-gfsad?qt-science_center_objects=4#qt-science_center_objects</t>
+  </si>
+  <si>
+    <t>Thenkabail, P., Knox, J., Ozdogan, M., Gumma, M., Congalton, R., Wu, Z., Milesi, C., Finkral, A., Marshall, M., Mariotto, I., You, S., Giri, C., Nagler, P. (2016). NASA Making Earth System Data Records for Use in Research Environments (MEaSUREs) Global Food Security Support Analysis Data (GFSAD) Crop Dominance 2010 Global 1 km V001 [Data set]. NASA EOSDIS Land Processes DAAC.</t>
+  </si>
+  <si>
+    <t>U.S. Census Grids: Summary File 1, v1</t>
+  </si>
+  <si>
+    <t>Gridded product including population totals from 2010 census at 1 km resolution. Separate files for contiguous USA, Hawaii, Alaska, and Aleutian islands</t>
+  </si>
+  <si>
+    <t>uspop10.tif, hipop10.tif, akpop10.tif, ehpop10.tif</t>
+  </si>
+  <si>
+    <t>https://sedac.ciesin.columbia.edu/data/set/usgrid-summary-file1-2010/data-download</t>
+  </si>
+  <si>
+    <t>Center For International Earth Science Information Network-CIESIN-Columbia University, 2017. U.S. Census Grids (Summary File 1), 2010. https://doi.org/10.7927/H40Z716C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +583,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -441,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -451,6 +627,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -732,9 +910,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -755,48 +933,48 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>2012</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2">
         <v>44278</v>
@@ -805,27 +983,27 @@
         <v>44278</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>2012</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2">
         <v>43762</v>
@@ -834,27 +1012,27 @@
         <v>44285</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>2012</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2">
         <v>43507</v>
@@ -863,27 +1041,27 @@
         <v>44285</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2">
         <v>43507</v>
@@ -892,27 +1070,27 @@
         <v>44285</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G6" s="2">
         <v>44172</v>
@@ -921,27 +1099,27 @@
         <v>44285</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G7" s="2">
         <v>44173</v>
@@ -950,27 +1128,27 @@
         <v>44285</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G8" s="2">
         <v>44174</v>
@@ -979,27 +1157,27 @@
         <v>44285</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9">
         <v>2010</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G9" s="2">
         <v>43538</v>
@@ -1008,27 +1186,27 @@
         <v>44285</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
         <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
       </c>
       <c r="G10" s="2">
         <v>44074</v>
@@ -1037,56 +1215,56 @@
         <v>44285</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="C11">
         <v>2012</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H11" s="2">
         <v>44285</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G12" s="2">
         <v>44172</v>
@@ -1095,15 +1273,313 @@
         <v>44285</v>
       </c>
       <c r="I12" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14">
+        <v>2009</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="2">
+        <v>43388</v>
+      </c>
+      <c r="H14" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15">
+        <v>2015</v>
+      </c>
+      <c r="D15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="2">
+        <v>42025</v>
+      </c>
+      <c r="H15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>2014</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="2">
+        <v>43069</v>
+      </c>
+      <c r="H16" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17">
+        <v>2020</v>
+      </c>
+      <c r="D17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="2">
+        <v>44090</v>
+      </c>
+      <c r="H17" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <v>2016</v>
+      </c>
+      <c r="D18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" s="2">
+        <v>43724</v>
+      </c>
+      <c r="H18" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19">
+        <v>2016</v>
+      </c>
+      <c r="D19" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="2">
+        <v>44231</v>
+      </c>
+      <c r="H19" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20">
+        <v>2001</v>
+      </c>
+      <c r="D20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="2">
+        <v>44231</v>
+      </c>
+      <c r="H20" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21">
+        <v>2000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" s="2">
+        <v>44090</v>
+      </c>
+      <c r="H21" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22">
+        <v>2010</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G22" s="2">
+        <v>44090</v>
+      </c>
+      <c r="H22" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23">
+        <v>2010</v>
+      </c>
+      <c r="D23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" t="s">
+        <v>177</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G23" s="2">
+        <v>44057</v>
+      </c>
+      <c r="H23" s="2">
+        <v>44284</v>
+      </c>
+      <c r="I23" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F12" r:id="rId1"/>
     <hyperlink ref="F11" r:id="rId2"/>
+    <hyperlink ref="F21" r:id="rId3"/>
+    <hyperlink ref="F22" r:id="rId4" location="qt-science_center_objects"/>
+    <hyperlink ref="F23" r:id="rId5"/>
+    <hyperlink ref="F14" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1111,7 +1587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1124,200 +1600,200 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" t="s">
         <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
         <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
       <c r="F9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small change to data source table
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_datasources.xlsx
+++ b/scenario_analysis_v2/scenariov2_datasources.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
   <si>
     <t>none (all data present in useeior package)</t>
   </si>
@@ -537,9 +537,6 @@
     <t>Ramankutty, N., Evan, A.T., Monfreda, C., Foley, J.A., 2008. Farming the planet: 1. Geographic distribution of global agricultural lands in the year 2000. Global Biogeochemical Cycles 22. https://doi.org/10.1029/2007GB002952</t>
   </si>
   <si>
-    <t>Global Food Security Support Analysis Data (GFSAD) Crop Dominance 2010 Global 1 km</t>
-  </si>
-  <si>
     <t>Raster at 1km resolution of global irrigated and rainfed cropland</t>
   </si>
   <si>
@@ -565,6 +562,12 @@
   </si>
   <si>
     <t>Center For International Earth Science Information Network-CIESIN-Columbia University, 2017. U.S. Census Grids (Summary File 1), 2010. https://doi.org/10.7927/H40Z716C</t>
+  </si>
+  <si>
+    <t>Global Food Security Support Analysis Data (GFSAD)</t>
+  </si>
+  <si>
+    <t>Crop Dominance 2010 Global 1 km</t>
   </si>
 </sst>
 </file>
@@ -913,7 +916,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,20 +1518,22 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B22"/>
+        <v>180</v>
+      </c>
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
       <c r="C22">
         <v>2010</v>
       </c>
       <c r="D22" t="s">
+        <v>170</v>
+      </c>
+      <c r="E22" t="s">
         <v>171</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="G22" s="2">
         <v>44090</v>
@@ -1537,12 +1542,12 @@
         <v>44284</v>
       </c>
       <c r="I22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B23" t="s">
         <v>165</v>
@@ -1551,13 +1556,13 @@
         <v>2010</v>
       </c>
       <c r="D23" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" t="s">
         <v>176</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="G23" s="2">
         <v>44057</v>
@@ -1566,7 +1571,7 @@
         <v>44284</v>
       </c>
       <c r="I23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data sources and pipeline
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_datasources.xlsx
+++ b/scenario_analysis_v2/scenariov2_datasources.xlsx
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="177">
   <si>
     <t>none (all data present in useeior package)</t>
   </si>
   <si>
-    <t>dietaryguidelinesfoodpatterns_cleaned.xlsx</t>
-  </si>
-  <si>
     <t>Dataset name</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>raw_data/Census/SUSB/us_state_6digitnaics_2012.txt</t>
   </si>
   <si>
-    <t>raw_data/commodity_flows/Lin_supp_info/County Personal Income.xlsx</t>
-  </si>
-  <si>
     <t>crossreference_tables/faostat_all_codes_harmonized.csv</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>multiple</t>
   </si>
   <si>
-    <t>https://www.dietaryguidelines.gov/sites/default/files/2019-05/2015-2020_Dietary_Guidelines.pdf</t>
-  </si>
-  <si>
     <t>https://www.nass.usda.gov/Publications/AgCensus/2012/Online_Resources/Census_Data_Query_Tool/2012_cdqt_data.txt.gz</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t>https://apps.bea.gov/iTable/iTable.cfm?reqid=70&amp;step=1&amp;acrdn=6</t>
   </si>
   <si>
-    <t>unknown</t>
-  </si>
-  <si>
     <t xml:space="preserve">FAOSTAT </t>
   </si>
   <si>
@@ -246,9 +234,6 @@
     <t>U.S. Census Bureau, 2015. SUSB Datasets [WWW Document]. The United States Census Bureau. URL https://www.census.gov/programs-surveys/susb/data/datasets.html (accessed 4.1.21).</t>
   </si>
   <si>
-    <t>U.S. Department of Health and Human Services, U.S. Department of Agriculture, 2015. 2015-2020 Dietary Guidelines for Americans, 8th Edition [WWW Document]. URL http://health.gov/dietaryguidelines/2015/guidelines (accessed 4.1.21).</t>
-  </si>
-  <si>
     <t>Willett, W., Rockström, J., Loken, B., Springmann, M., Lang, T., Vermeulen, S., Garnett, T., Tilman, D., DeClerck, F., Wood, A., Jonell, M., Clark, M., Gordon, L.J., Fanzo, J., Hawkes, C., Zurayk, R., Rivera, J.A., De Vries, W., Majele Sibanda, L., Afshin, A., Chaudhary, A., Herrero, M., Agustina, R., Branca, F., Lartey, A., Fan, S., Crona, B., Fox, E., Bignet, V., Troell, M., Lindahl, T., Singh, S., Cornell, S.E., Srinath Reddy, K., Narain, S., Nishtar, S., Murray, C.J.L., 2019. Food in the Anthropocene: the EAT–Lancet Commission on healthy diets from sustainable food systems. The Lancet 393, 447–492. https://doi.org/10.1016/S0140-6736(18)31788-4</t>
   </si>
   <si>
@@ -420,27 +405,9 @@
     <t>Olson, D. M. and E. Dinerstein. 2002. The Global 200: Priority ecoregions for global conservation. (PDF file) Annals of the Missouri Botanical Garden 89:125-126.</t>
   </si>
   <si>
-    <t>United States administrative boundaries shapefile</t>
-  </si>
-  <si>
-    <t>Global Administrative Areas Database</t>
-  </si>
-  <si>
-    <t>Polygon file of the United States' country boundaries based on GADM v2.0</t>
-  </si>
-  <si>
-    <t>USA_adm0.shp (ESRI shapefile with multiple files)</t>
-  </si>
-  <si>
-    <t>No longer available. The most recent version is available at https://gadm.org/download_country_v3.html</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>GADM (Global Administrative Areas Database) [WWW Document], n.d. URL https://gadm.org/ (accessed 4.1.21).</t>
-  </si>
-  <si>
     <t>United States county boundaries shapefile</t>
   </si>
   <si>
@@ -568,6 +535,27 @@
   </si>
   <si>
     <t>Crop Dominance 2010 Global 1 km</t>
+  </si>
+  <si>
+    <t>raw_data/BEA/countypersonalincome2012.csv</t>
+  </si>
+  <si>
+    <t>FIPS codes harmonization between Census Tiger shapefile and county personal income data</t>
+  </si>
+  <si>
+    <t>crossreference_tables/fips_harmonization.csv</t>
+  </si>
+  <si>
+    <t>For combining map polygons of county map to match the income data otherwise used to downscale data to county level</t>
+  </si>
+  <si>
+    <t>dietaryguidelines2020-2025cleaned.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.dietaryguidelines.gov/sites/default/files/2021-03/Dietary_Guidelines_for_Americans-2020-2025.pdf</t>
+  </si>
+  <si>
+    <t>U.S. Department of Health and Human Services, U.S. Department of Agriculture, 2020. Dietary Guidelines for Americans, 2020-2025 [WWW Document].</t>
   </si>
 </sst>
 </file>
@@ -913,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,51 +921,51 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>2012</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2">
         <v>44278</v>
@@ -986,27 +974,27 @@
         <v>44278</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>2012</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G3" s="2">
         <v>43762</v>
@@ -1015,27 +1003,27 @@
         <v>44285</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>2012</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2">
         <v>43507</v>
@@ -1044,27 +1032,27 @@
         <v>44285</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2">
         <v>43507</v>
@@ -1073,56 +1061,56 @@
         <v>44285</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
+        <v>174</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="G6" s="2">
-        <v>44172</v>
+        <v>44306</v>
       </c>
       <c r="H6" s="2">
-        <v>44285</v>
+        <v>44306</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2">
         <v>44173</v>
@@ -1131,27 +1119,27 @@
         <v>44285</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2">
         <v>44174</v>
@@ -1160,27 +1148,27 @@
         <v>44285</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>2010</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G9" s="2">
         <v>43538</v>
@@ -1189,27 +1177,27 @@
         <v>44285</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
         <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
       </c>
       <c r="G10" s="2">
         <v>44074</v>
@@ -1218,56 +1206,56 @@
         <v>44285</v>
       </c>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C11">
         <v>2012</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="G11" s="2">
+        <v>44305</v>
       </c>
       <c r="H11" s="2">
-        <v>44285</v>
+        <v>44305</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G12" s="2">
         <v>44172</v>
@@ -1276,32 +1264,32 @@
         <v>44285</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C14">
         <v>2009</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G14" s="2">
         <v>43388</v>
@@ -1310,143 +1298,143 @@
         <v>44284</v>
       </c>
       <c r="I14" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>2014</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="2">
+        <v>43069</v>
+      </c>
+      <c r="H15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" t="s">
         <v>131</v>
-      </c>
-      <c r="B15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15">
-        <v>2015</v>
-      </c>
-      <c r="D15" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="2">
-        <v>42025</v>
-      </c>
-      <c r="H15" t="s">
-        <v>136</v>
-      </c>
-      <c r="I15" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="C16">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G16" s="2">
-        <v>43069</v>
-      </c>
-      <c r="H16" t="s">
-        <v>136</v>
+        <v>44090</v>
+      </c>
+      <c r="H16" s="2">
+        <v>44284</v>
       </c>
       <c r="I16" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C17">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G17" s="2">
-        <v>44090</v>
+        <v>43724</v>
       </c>
       <c r="H17" s="2">
         <v>44284</v>
       </c>
       <c r="I17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C18">
         <v>2016</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G18" s="2">
-        <v>43724</v>
+        <v>44231</v>
       </c>
       <c r="H18" s="2">
         <v>44284</v>
       </c>
       <c r="I18" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19">
+        <v>2001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" t="s">
         <v>150</v>
       </c>
-      <c r="C19">
-        <v>2016</v>
-      </c>
-      <c r="D19" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" t="s">
-        <v>157</v>
-      </c>
       <c r="F19" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G19" s="2">
         <v>44231</v>
@@ -1455,56 +1443,56 @@
         <v>44284</v>
       </c>
       <c r="I19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C20">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
-        <v>161</v>
-      </c>
-      <c r="F20" t="s">
-        <v>162</v>
+        <v>156</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="G20" s="2">
-        <v>44231</v>
+        <v>44090</v>
       </c>
       <c r="H20" s="2">
         <v>44284</v>
       </c>
       <c r="I20" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C21">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>167</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="G21" s="2">
         <v>44090</v>
@@ -1513,87 +1501,59 @@
         <v>44284</v>
       </c>
       <c r="I21" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="C22">
         <v>2010</v>
       </c>
       <c r="D22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E22" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G22" s="2">
-        <v>44090</v>
+        <v>44057</v>
       </c>
       <c r="H22" s="2">
         <v>44284</v>
       </c>
       <c r="I22" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23">
-        <v>2010</v>
-      </c>
-      <c r="D23" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="G23" s="2">
-        <v>44057</v>
-      </c>
-      <c r="H23" s="2">
-        <v>44284</v>
-      </c>
-      <c r="I23" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F12" r:id="rId1"/>
     <hyperlink ref="F11" r:id="rId2"/>
-    <hyperlink ref="F21" r:id="rId3"/>
-    <hyperlink ref="F22" r:id="rId4" location="qt-science_center_objects"/>
-    <hyperlink ref="F23" r:id="rId5"/>
+    <hyperlink ref="F20" r:id="rId3"/>
+    <hyperlink ref="F21" r:id="rId4" location="qt-science_center_objects"/>
+    <hyperlink ref="F22" r:id="rId5"/>
     <hyperlink ref="F14" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,200 +1565,214 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
         <v>94</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
         <v>81</v>
       </c>
-      <c r="C12" t="s">
-        <v>86</v>
-      </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>